<commit_message>
Hecho correcciones de Profes TP12
</commit_message>
<xml_diff>
--- a/Trabajos_practicos/Trabajo_practico_12_Testing-Ejecucion_de_Casos_de_Prueba-E/Trabajo_Practico_12_Grupo6.xlsx
+++ b/Trabajos_practicos/Trabajo_practico_12_Testing-Ejecucion_de_Casos_de_Prueba-E/Trabajo_Practico_12_Grupo6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo Paz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo Paz\Documents\3-Uni\General\4toAño\ISW4K1\Repo\Ingenieria_de_software_2021-Grupo_6\Trabajos_practicos\Trabajo_practico_12_Testing-Ejecucion_de_Casos_de_Prueba-E\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A28356-80E4-4471-86C6-E3FB51AEAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA73FC-86BC-458F-AF06-445DEF909BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="1" r:id="rId1"/>
@@ -2197,6 +2197,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2219,11 +2230,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2235,12 +2241,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2790,9 +2790,9 @@
   </sheetPr>
   <dimension ref="A1:AP963"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1"/>
@@ -2867,14 +2867,14 @@
       <c r="AP1" s="3"/>
     </row>
     <row r="2" spans="1:42" ht="12.75" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="83"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="4"/>
@@ -2913,12 +2913,12 @@
       <c r="AP2" s="3"/>
     </row>
     <row r="3" spans="1:42" ht="12.75" customHeight="1">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="81"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="4"/>
@@ -2957,12 +2957,12 @@
       <c r="AP3" s="3"/>
     </row>
     <row r="4" spans="1:42" ht="12.75" customHeight="1">
-      <c r="A4" s="82"/>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="84"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="I4" s="4"/>
@@ -3001,16 +3001,16 @@
       <c r="AP4" s="3"/>
     </row>
     <row r="5" spans="1:42" ht="12.75" customHeight="1">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="86"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="87"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="86"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="91"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="7"/>
@@ -3141,34 +3141,34 @@
       <c r="AP7" s="3"/>
     </row>
     <row r="8" spans="1:42" ht="12.75" customHeight="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="92" t="s">
+      <c r="A8" s="94"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="92" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="92" t="s">
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="90"/>
-      <c r="T8" s="90"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="91"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="80"/>
       <c r="W8" s="18"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -3803,9 +3803,7 @@
         <v>28</v>
       </c>
       <c r="J18" s="45"/>
-      <c r="K18" s="46">
-        <v>4</v>
-      </c>
+      <c r="K18" s="46"/>
       <c r="L18" s="52">
         <v>44481</v>
       </c>
@@ -46043,8 +46041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H990"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1"/>
@@ -46117,7 +46115,7 @@
       <c r="D4" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="76" t="s">
         <v>253</v>
       </c>
       <c r="F4" s="44" t="s">
@@ -46187,7 +46185,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="44">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C7" s="65">
         <v>44481</v>
@@ -46221,7 +46219,7 @@
       <c r="D8" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="77" t="s">
         <v>254</v>
       </c>
       <c r="F8" s="44" t="s">
@@ -47257,23 +47255,23 @@
       <c r="A1" s="68" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="95" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="97" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="94"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="94"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="96"/>
     </row>
     <row r="3" spans="1:5" ht="30.75" customHeight="1">
       <c r="A3" s="69" t="s">
@@ -47616,13 +47614,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="98" t="s">
         <v>241</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="94"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="96"/>
     </row>
     <row r="28" spans="1:5" ht="30.75" customHeight="1">
       <c r="A28" s="69" t="s">

</xml_diff>